<commit_message>
Änderungen vom Labor (SW Test, ...)
</commit_message>
<xml_diff>
--- a/Übersicht.xlsx
+++ b/Übersicht.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="106" uniqueCount="38">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="136" uniqueCount="38">
   <si>
     <t>Bezeichnung</t>
   </si>
@@ -621,7 +621,7 @@
   <dimension ref="A1:K18"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="I11" sqref="I11"/>
+      <selection activeCell="I22" sqref="I22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -933,14 +933,28 @@
       <c r="B11" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="C11" s="2"/>
-      <c r="D11" s="2"/>
-      <c r="E11" s="2"/>
-      <c r="F11" s="2"/>
-      <c r="G11" s="2"/>
-      <c r="H11" s="2"/>
+      <c r="C11" s="12" t="s">
+        <v>35</v>
+      </c>
+      <c r="D11" s="12" t="s">
+        <v>35</v>
+      </c>
+      <c r="E11" s="12" t="s">
+        <v>35</v>
+      </c>
+      <c r="F11" s="12" t="s">
+        <v>35</v>
+      </c>
+      <c r="G11" s="12" t="s">
+        <v>35</v>
+      </c>
+      <c r="H11" s="12" t="s">
+        <v>35</v>
+      </c>
       <c r="I11" s="2"/>
-      <c r="J11" s="2"/>
+      <c r="J11" s="12" t="s">
+        <v>35</v>
+      </c>
       <c r="K11" s="2"/>
     </row>
     <row r="12" spans="1:11" s="6" customFormat="1" ht="15" x14ac:dyDescent="0.2">
@@ -972,15 +986,27 @@
       <c r="C13" s="7" t="s">
         <v>35</v>
       </c>
-      <c r="D13" s="2"/>
-      <c r="E13" s="2"/>
-      <c r="F13" s="2"/>
+      <c r="D13" s="12" t="s">
+        <v>35</v>
+      </c>
+      <c r="E13" s="12" t="s">
+        <v>35</v>
+      </c>
+      <c r="F13" s="12" t="s">
+        <v>35</v>
+      </c>
       <c r="G13" s="7" t="s">
         <v>35</v>
       </c>
-      <c r="H13" s="2"/>
-      <c r="I13" s="2"/>
-      <c r="J13" s="2"/>
+      <c r="H13" s="12" t="s">
+        <v>35</v>
+      </c>
+      <c r="I13" s="12" t="s">
+        <v>35</v>
+      </c>
+      <c r="J13" s="12" t="s">
+        <v>35</v>
+      </c>
       <c r="K13" s="1"/>
     </row>
     <row r="14" spans="1:11" ht="15" x14ac:dyDescent="0.2">
@@ -993,13 +1019,21 @@
       <c r="C14" s="7" t="s">
         <v>35</v>
       </c>
-      <c r="D14" s="2"/>
-      <c r="E14" s="2"/>
-      <c r="F14" s="2"/>
+      <c r="D14" s="12" t="s">
+        <v>35</v>
+      </c>
+      <c r="E14" s="12" t="s">
+        <v>35</v>
+      </c>
+      <c r="F14" s="12" t="s">
+        <v>35</v>
+      </c>
       <c r="G14" s="7" t="s">
         <v>35</v>
       </c>
-      <c r="H14" s="2"/>
+      <c r="H14" s="12" t="s">
+        <v>35</v>
+      </c>
       <c r="I14" s="2"/>
       <c r="J14" s="2"/>
       <c r="K14" s="2"/>
@@ -1012,13 +1046,21 @@
       <c r="C15" s="7" t="s">
         <v>35</v>
       </c>
-      <c r="D15" s="2"/>
-      <c r="E15" s="2"/>
-      <c r="F15" s="2"/>
+      <c r="D15" s="12" t="s">
+        <v>35</v>
+      </c>
+      <c r="E15" s="12" t="s">
+        <v>35</v>
+      </c>
+      <c r="F15" s="12" t="s">
+        <v>35</v>
+      </c>
       <c r="G15" s="7" t="s">
         <v>35</v>
       </c>
-      <c r="H15" s="2"/>
+      <c r="H15" s="12" t="s">
+        <v>35</v>
+      </c>
       <c r="I15" s="2"/>
       <c r="J15" s="2"/>
       <c r="K15" s="2"/>
@@ -1033,13 +1075,21 @@
       <c r="C16" s="7" t="s">
         <v>35</v>
       </c>
-      <c r="D16" s="2"/>
-      <c r="E16" s="2"/>
-      <c r="F16" s="2"/>
+      <c r="D16" s="12" t="s">
+        <v>35</v>
+      </c>
+      <c r="E16" s="12" t="s">
+        <v>35</v>
+      </c>
+      <c r="F16" s="12" t="s">
+        <v>35</v>
+      </c>
       <c r="G16" s="7" t="s">
         <v>35</v>
       </c>
-      <c r="H16" s="2"/>
+      <c r="H16" s="12" t="s">
+        <v>35</v>
+      </c>
       <c r="I16" s="2"/>
       <c r="J16" s="2"/>
       <c r="K16" s="2"/>
@@ -1052,13 +1102,21 @@
       <c r="C17" s="7" t="s">
         <v>35</v>
       </c>
-      <c r="D17" s="2"/>
-      <c r="E17" s="2"/>
-      <c r="F17" s="2"/>
+      <c r="D17" s="12" t="s">
+        <v>35</v>
+      </c>
+      <c r="E17" s="12" t="s">
+        <v>35</v>
+      </c>
+      <c r="F17" s="12" t="s">
+        <v>35</v>
+      </c>
       <c r="G17" s="7" t="s">
         <v>35</v>
       </c>
-      <c r="H17" s="2"/>
+      <c r="H17" s="12" t="s">
+        <v>35</v>
+      </c>
       <c r="I17" s="2"/>
       <c r="J17" s="2"/>
       <c r="K17" s="2"/>
@@ -1079,7 +1137,9 @@
       <c r="G18" s="7" t="s">
         <v>35</v>
       </c>
-      <c r="H18" s="2"/>
+      <c r="H18" s="12" t="s">
+        <v>35</v>
+      </c>
       <c r="I18" s="2"/>
       <c r="J18" s="2"/>
       <c r="K18" s="2"/>

</xml_diff>